<commit_message>
Foram feitas algumas modificações na escrita e exibição de alguns itens
</commit_message>
<xml_diff>
--- a/src/Ramais.xlsx
+++ b/src/Ramais.xlsx
@@ -519,7 +519,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">PABX </t>
+          <t>PABX</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -22476,7 +22476,7 @@
       </c>
       <c r="K354" t="inlineStr">
         <is>
-          <t>s</t>
+          <t>P</t>
         </is>
       </c>
       <c r="L354" t="inlineStr">
@@ -22549,7 +22549,7 @@
       </c>
       <c r="K355" t="inlineStr">
         <is>
-          <t>s</t>
+          <t>P</t>
         </is>
       </c>
       <c r="L355" t="inlineStr">

</xml_diff>

<commit_message>
Inclusão de labels para tornar mais claro o que cada coisa faz]
</commit_message>
<xml_diff>
--- a/src/Ramais.xlsx
+++ b/src/Ramais.xlsx
@@ -597,7 +597,7 @@
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Superintendencia</t>
+          <t>SUPERINTENDÊNCIA</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -662,7 +662,7 @@
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Superintendencia</t>
+          <t>SUPERINTENDÊNCIA</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -990,12 +990,12 @@
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Suporte Operacional </t>
+          <t>SUPORTE OPERACIONAL</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Protocolo</t>
+          <t>PROTOCOLO</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -1059,12 +1059,12 @@
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Externo</t>
+          <t>EXTERNO</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Auditoria Municipal </t>
+          <t>AUDITORIA MUNICIPAL</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1120,12 +1120,12 @@
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Externo</t>
+          <t>EXTERNO</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Lanchonete </t>
+          <t>LANCHONETE</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1181,12 +1181,12 @@
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Externo</t>
+          <t>EXTERNO</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Jurídico</t>
+          <t>JURÍDICO</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1242,12 +1242,12 @@
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Setor de contratualização e Regularização</t>
+          <t>SETOR DE CONTRATUALIZAÇÃO E REGULAÇÃO</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Setor de contratualização e Regularização</t>
+          <t>SETOR DE CONTRATUALIZAÇÃO E REGULAÇÃO</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -3643,7 +3643,7 @@
       <c r="G53" t="inlineStr"/>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Superintendencia</t>
+          <t>SUPERINTENDÊNCIA</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
@@ -3700,7 +3700,7 @@
       <c r="G54" t="inlineStr"/>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Superintendencia</t>
+          <t>SUPERINTENDÊNCIA</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
@@ -3757,7 +3757,7 @@
       <c r="G55" t="inlineStr"/>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Superintendencia</t>
+          <t>SUPERINTENDÊNCIA</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
@@ -3814,7 +3814,7 @@
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Superintendencia</t>
+          <t>SUPERINTENDÊNCIA</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
@@ -3871,7 +3871,7 @@
       <c r="G57" t="inlineStr"/>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Superintendencia</t>
+          <t>SUPERINTENDÊNCIA</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
@@ -3928,7 +3928,7 @@
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Superintendencia</t>
+          <t>SUPERINTENDÊNCIA</t>
         </is>
       </c>
       <c r="I58" t="inlineStr">
@@ -3985,7 +3985,7 @@
       <c r="G59" t="inlineStr"/>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Superintendencia</t>
+          <t>SUPERINTENDÊNCIA</t>
         </is>
       </c>
       <c r="I59" t="inlineStr">
@@ -4042,7 +4042,7 @@
       <c r="G60" t="inlineStr"/>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Superintendencia</t>
+          <t>SUPERINTENDÊNCIA</t>
         </is>
       </c>
       <c r="I60" t="inlineStr">
@@ -4099,7 +4099,7 @@
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Superintendencia</t>
+          <t>SUPERINTENDÊNCIA</t>
         </is>
       </c>
       <c r="I61" t="inlineStr">
@@ -4156,7 +4156,7 @@
       <c r="G62" t="inlineStr"/>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Superintendencia</t>
+          <t>SUPERINTENDÊNCIA</t>
         </is>
       </c>
       <c r="I62" t="inlineStr">
@@ -4213,7 +4213,7 @@
       <c r="G63" t="inlineStr"/>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Superintendencia</t>
+          <t>SUPERINTENDÊNCIA</t>
         </is>
       </c>
       <c r="I63" t="inlineStr">
@@ -4270,7 +4270,7 @@
       <c r="G64" t="inlineStr"/>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Superintendencia</t>
+          <t>SUPERINTENDÊNCIA</t>
         </is>
       </c>
       <c r="I64" t="inlineStr">
@@ -4327,7 +4327,7 @@
       <c r="G65" t="inlineStr"/>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Superintendencia</t>
+          <t>SUPERINTENDÊNCIA</t>
         </is>
       </c>
       <c r="I65" t="inlineStr">
@@ -4383,12 +4383,12 @@
       <c r="F66" t="inlineStr"/>
       <c r="G66" t="inlineStr">
         <is>
-          <t>Faturamento Hospitalar</t>
+          <t>FATURAMENTO HOSPITALAR</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Faturamento Hospitalar</t>
+          <t>FATURAMENTO HOSPITALAR</t>
         </is>
       </c>
       <c r="I66" t="inlineStr">
@@ -4623,8 +4623,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t xml:space="preserve">Chefia UDIS
-</t>
+          <t>Chefia UDIS</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -7281,7 +7280,7 @@
       </c>
       <c r="H110" t="inlineStr">
         <is>
-          <t>Unidade de Nutrição clinica</t>
+          <t>UNIDADE DE NUTRIÇÃO CLÍNICA</t>
         </is>
       </c>
       <c r="I110" t="inlineStr">
@@ -7346,7 +7345,7 @@
       </c>
       <c r="H111" t="inlineStr">
         <is>
-          <t>Unidade de Nutrição clinica</t>
+          <t>UNIDADE DE NUTRIÇÃO CLÍNICA</t>
         </is>
       </c>
       <c r="I111" t="inlineStr">
@@ -7411,7 +7410,7 @@
       </c>
       <c r="H112" t="inlineStr">
         <is>
-          <t>Unidade de Nutrição clinica</t>
+          <t>UNIDADE DE NUTRIÇÃO CLÍNICA</t>
         </is>
       </c>
       <c r="I112" t="inlineStr">
@@ -7476,7 +7475,7 @@
       </c>
       <c r="H113" t="inlineStr">
         <is>
-          <t>Unidade de Nutrição clinica</t>
+          <t>UNIDADE DE NUTRIÇÃO CLÍNICA</t>
         </is>
       </c>
       <c r="I113" t="inlineStr">
@@ -7541,7 +7540,7 @@
       </c>
       <c r="H114" t="inlineStr">
         <is>
-          <t>Unidade de Nutrição clinica</t>
+          <t>UNIDADE DE NUTRIÇÃO CLÍNICA</t>
         </is>
       </c>
       <c r="I114" t="inlineStr">
@@ -8408,7 +8407,7 @@
       </c>
       <c r="H127" t="inlineStr">
         <is>
-          <t>Morgue</t>
+          <t>MORGE</t>
         </is>
       </c>
       <c r="I127" t="inlineStr">
@@ -11647,8 +11646,7 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t xml:space="preserve"> UMC-T-Recepcao-Maternidade
-</t>
+          <t xml:space="preserve"> UMC-T-Recepcao-Maternidade</t>
         </is>
       </c>
       <c r="D179" t="inlineStr">
@@ -13180,7 +13178,7 @@
       <c r="G202" t="inlineStr"/>
       <c r="H202" t="inlineStr">
         <is>
-          <t>Unidade de Apoio à Gestão em Enfermagem</t>
+          <t>UNIDADE DE APOIO Á GESTÃO EM INFERMAGEM</t>
         </is>
       </c>
       <c r="I202" t="inlineStr">
@@ -13241,7 +13239,7 @@
       <c r="G203" t="inlineStr"/>
       <c r="H203" t="inlineStr">
         <is>
-          <t>Unidade de Apoio à Gestão em Enfermagem</t>
+          <t>UNIDADE DE APOIO Á GESTÃO EM INFERMAGEM</t>
         </is>
       </c>
       <c r="I203" t="inlineStr">
@@ -13302,7 +13300,7 @@
       <c r="G204" t="inlineStr"/>
       <c r="H204" t="inlineStr">
         <is>
-          <t>Unidade de Apoio à Gestão em Enfermagem</t>
+          <t>UNIDADE DE APOIO Á GESTÃO EM INFERMAGEM</t>
         </is>
       </c>
       <c r="I204" t="inlineStr">
@@ -13363,7 +13361,7 @@
       <c r="G205" t="inlineStr"/>
       <c r="H205" t="inlineStr">
         <is>
-          <t>Unidade de Apoio à Gestão em Enfermagem</t>
+          <t>UNIDADE DE APOIO Á GESTÃO EM INFERMAGEM</t>
         </is>
       </c>
       <c r="I205" t="inlineStr">
@@ -15683,7 +15681,7 @@
       </c>
       <c r="H241" t="inlineStr">
         <is>
-          <t>Unidade de Almoxarifado e Controle de estoques</t>
+          <t>UNIDADE DE ALMOXARIFADO E CONTROLE DE ESTOQUES</t>
         </is>
       </c>
       <c r="I241" t="inlineStr">
@@ -15748,7 +15746,7 @@
       </c>
       <c r="H242" t="inlineStr">
         <is>
-          <t>Unidade de Almoxarifado e Controle de estoques</t>
+          <t>UNIDADE DE ALMOXARIFADO E CONTROLE DE ESTOQUES</t>
         </is>
       </c>
       <c r="I242" t="inlineStr">
@@ -15813,7 +15811,7 @@
       </c>
       <c r="H243" t="inlineStr">
         <is>
-          <t>Unidade de Almoxarifado e Controle de estoques</t>
+          <t>UNIDADE DE ALMOXARIFADO E CONTROLE DE ESTOQUES</t>
         </is>
       </c>
       <c r="I243" t="inlineStr">
@@ -15878,7 +15876,7 @@
       </c>
       <c r="H244" t="inlineStr">
         <is>
-          <t>Unidade de Almoxarifado e Controle de estoques</t>
+          <t>UNIDADE DE ALMOXARIFADO E CONTROLE DE ESTOQUES</t>
         </is>
       </c>
       <c r="I244" t="inlineStr">
@@ -19669,12 +19667,12 @@
       <c r="F304" t="inlineStr"/>
       <c r="G304" t="inlineStr">
         <is>
-          <t xml:space="preserve">Suporte Operacional </t>
+          <t>SUPORTE OPERACIONAL</t>
         </is>
       </c>
       <c r="H304" t="inlineStr">
         <is>
-          <t xml:space="preserve">Suporte Operacional </t>
+          <t>SUPORTE OPERACIONAL</t>
         </is>
       </c>
       <c r="I304" t="inlineStr">
@@ -19730,12 +19728,12 @@
       <c r="F305" t="inlineStr"/>
       <c r="G305" t="inlineStr">
         <is>
-          <t xml:space="preserve">Suporte Operacional </t>
+          <t>SUPORTE OPERACIONAL</t>
         </is>
       </c>
       <c r="H305" t="inlineStr">
         <is>
-          <t xml:space="preserve">Suporte Operacional </t>
+          <t>SUPORTE OPERACIONAL</t>
         </is>
       </c>
       <c r="I305" t="inlineStr">
@@ -19791,12 +19789,12 @@
       <c r="F306" t="inlineStr"/>
       <c r="G306" t="inlineStr">
         <is>
-          <t xml:space="preserve">Suporte Operacional </t>
+          <t>SUPORTE OPERACIONAL</t>
         </is>
       </c>
       <c r="H306" t="inlineStr">
         <is>
-          <t xml:space="preserve">Suporte Operacional </t>
+          <t>SUPORTE OPERACIONAL</t>
         </is>
       </c>
       <c r="I306" t="inlineStr">
@@ -19852,12 +19850,12 @@
       <c r="F307" t="inlineStr"/>
       <c r="G307" t="inlineStr">
         <is>
-          <t xml:space="preserve">Suporte Operacional </t>
+          <t>SUPORTE OPERACIONAL</t>
         </is>
       </c>
       <c r="H307" t="inlineStr">
         <is>
-          <t>Guarita</t>
+          <t>GUARITA</t>
         </is>
       </c>
       <c r="I307" t="inlineStr">
@@ -19913,12 +19911,12 @@
       <c r="F308" t="inlineStr"/>
       <c r="G308" t="inlineStr">
         <is>
-          <t xml:space="preserve">Suporte Operacional </t>
+          <t>SUPORTE OPERACIONAL</t>
         </is>
       </c>
       <c r="H308" t="inlineStr">
         <is>
-          <t>transporte administrativo</t>
+          <t>TRANSPORTES</t>
         </is>
       </c>
       <c r="I308" t="inlineStr">
@@ -19974,12 +19972,12 @@
       <c r="F309" t="inlineStr"/>
       <c r="G309" t="inlineStr">
         <is>
-          <t xml:space="preserve">Suporte Operacional </t>
+          <t>SUPORTE OPERACIONAL</t>
         </is>
       </c>
       <c r="H309" t="inlineStr">
         <is>
-          <t>recepções</t>
+          <t>RECEPÇÕES</t>
         </is>
       </c>
       <c r="I309" t="inlineStr">
@@ -20035,12 +20033,12 @@
       <c r="F310" t="inlineStr"/>
       <c r="G310" t="inlineStr">
         <is>
-          <t xml:space="preserve">Suporte Operacional </t>
+          <t>SUPORTE OPERACIONAL</t>
         </is>
       </c>
       <c r="H310" t="inlineStr">
         <is>
-          <t>recepções</t>
+          <t>RECEPÇÕES</t>
         </is>
       </c>
       <c r="I310" t="inlineStr">
@@ -20096,12 +20094,12 @@
       <c r="F311" t="inlineStr"/>
       <c r="G311" t="inlineStr">
         <is>
-          <t xml:space="preserve">Suporte Operacional </t>
+          <t>SUPORTE OPERACIONAL</t>
         </is>
       </c>
       <c r="H311" t="inlineStr">
         <is>
-          <t>recepções</t>
+          <t>RECEPÇÕES</t>
         </is>
       </c>
       <c r="I311" t="inlineStr">
@@ -20157,12 +20155,12 @@
       <c r="F312" t="inlineStr"/>
       <c r="G312" t="inlineStr">
         <is>
-          <t xml:space="preserve">Suporte Operacional </t>
+          <t>SUPORTE OPERACIONAL</t>
         </is>
       </c>
       <c r="H312" t="inlineStr">
         <is>
-          <t>recepções</t>
+          <t>RECEPÇÕES</t>
         </is>
       </c>
       <c r="I312" t="inlineStr">
@@ -20218,12 +20216,12 @@
       <c r="F313" t="inlineStr"/>
       <c r="G313" t="inlineStr">
         <is>
-          <t xml:space="preserve">Suporte Operacional </t>
+          <t>SUPORTE OPERACIONAL</t>
         </is>
       </c>
       <c r="H313" t="inlineStr">
         <is>
-          <t>recepções</t>
+          <t>RECEPÇÕES</t>
         </is>
       </c>
       <c r="I313" t="inlineStr">
@@ -20279,12 +20277,12 @@
       <c r="F314" t="inlineStr"/>
       <c r="G314" t="inlineStr">
         <is>
-          <t xml:space="preserve">Suporte Operacional </t>
+          <t>SUPORTE OPERACIONAL</t>
         </is>
       </c>
       <c r="H314" t="inlineStr">
         <is>
-          <t>recepções</t>
+          <t>RECEPÇÕES</t>
         </is>
       </c>
       <c r="I314" t="inlineStr">
@@ -20340,12 +20338,12 @@
       <c r="F315" t="inlineStr"/>
       <c r="G315" t="inlineStr">
         <is>
-          <t xml:space="preserve">Suporte Operacional </t>
+          <t>SUPORTE OPERACIONAL</t>
         </is>
       </c>
       <c r="H315" t="inlineStr">
         <is>
-          <t>recepções</t>
+          <t>RECEPÇÕES</t>
         </is>
       </c>
       <c r="I315" t="inlineStr">
@@ -20401,12 +20399,12 @@
       <c r="F316" t="inlineStr"/>
       <c r="G316" t="inlineStr">
         <is>
-          <t xml:space="preserve">Suporte Operacional </t>
+          <t>SUPORTE OPERACIONAL</t>
         </is>
       </c>
       <c r="H316" t="inlineStr">
         <is>
-          <t>recepções</t>
+          <t>RECEPÇÕES</t>
         </is>
       </c>
       <c r="I316" t="inlineStr">
@@ -20462,12 +20460,12 @@
       <c r="F317" t="inlineStr"/>
       <c r="G317" t="inlineStr">
         <is>
-          <t xml:space="preserve">Suporte Operacional </t>
+          <t>SUPORTE OPERACIONAL</t>
         </is>
       </c>
       <c r="H317" t="inlineStr">
         <is>
-          <t>recepções</t>
+          <t>RECEPÇÕES</t>
         </is>
       </c>
       <c r="I317" t="inlineStr">
@@ -20523,12 +20521,12 @@
       <c r="F318" t="inlineStr"/>
       <c r="G318" t="inlineStr">
         <is>
-          <t xml:space="preserve">Suporte Operacional </t>
+          <t>SUPORTE OPERACIONAL</t>
         </is>
       </c>
       <c r="H318" t="inlineStr">
         <is>
-          <t>recepções</t>
+          <t>RECEPÇÕES</t>
         </is>
       </c>
       <c r="I318" t="inlineStr">
@@ -20584,12 +20582,12 @@
       <c r="F319" t="inlineStr"/>
       <c r="G319" t="inlineStr">
         <is>
-          <t xml:space="preserve">Suporte Operacional </t>
+          <t>SUPORTE OPERACIONAL</t>
         </is>
       </c>
       <c r="H319" t="inlineStr">
         <is>
-          <t>recepções</t>
+          <t>RECEPÇÕES</t>
         </is>
       </c>
       <c r="I319" t="inlineStr">
@@ -20645,12 +20643,12 @@
       <c r="F320" t="inlineStr"/>
       <c r="G320" t="inlineStr">
         <is>
-          <t xml:space="preserve">Suporte Operacional </t>
+          <t>SUPORTE OPERACIONAL</t>
         </is>
       </c>
       <c r="H320" t="inlineStr">
         <is>
-          <t>recepções</t>
+          <t>RECEPÇÕES</t>
         </is>
       </c>
       <c r="I320" t="inlineStr">
@@ -20706,12 +20704,12 @@
       <c r="F321" t="inlineStr"/>
       <c r="G321" t="inlineStr">
         <is>
-          <t xml:space="preserve">Suporte Operacional </t>
+          <t>SUPORTE OPERACIONAL</t>
         </is>
       </c>
       <c r="H321" t="inlineStr">
         <is>
-          <t>recepções</t>
+          <t>RECEPÇÕES</t>
         </is>
       </c>
       <c r="I321" t="inlineStr">
@@ -20767,12 +20765,12 @@
       <c r="F322" t="inlineStr"/>
       <c r="G322" t="inlineStr">
         <is>
-          <t xml:space="preserve">Suporte Operacional </t>
+          <t>SUPORTE OPERACIONAL</t>
         </is>
       </c>
       <c r="H322" t="inlineStr">
         <is>
-          <t>recepções</t>
+          <t>RECEPÇÕES</t>
         </is>
       </c>
       <c r="I322" t="inlineStr">
@@ -20828,12 +20826,12 @@
       <c r="F323" t="inlineStr"/>
       <c r="G323" t="inlineStr">
         <is>
-          <t xml:space="preserve">Suporte Operacional </t>
+          <t>SUPORTE OPERACIONAL</t>
         </is>
       </c>
       <c r="H323" t="inlineStr">
         <is>
-          <t>recepções</t>
+          <t>RECEPÇÕES</t>
         </is>
       </c>
       <c r="I323" t="inlineStr">
@@ -21876,7 +21874,7 @@
       </c>
       <c r="E341" t="inlineStr">
         <is>
-          <t>Superintendencia</t>
+          <t>SUPERINTENDÊNCIA</t>
         </is>
       </c>
       <c r="F341" t="inlineStr"/>
@@ -21896,7 +21894,11 @@
           <t>n</t>
         </is>
       </c>
-      <c r="K341" t="inlineStr"/>
+      <c r="K341" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="L341" t="inlineStr"/>
       <c r="M341" t="inlineStr"/>
       <c r="N341" t="inlineStr">
@@ -22249,7 +22251,7 @@
       <c r="D350" t="inlineStr"/>
       <c r="E350" t="inlineStr">
         <is>
-          <t>Superintendencia</t>
+          <t>SUPERINTENDÊNCIA</t>
         </is>
       </c>
       <c r="F350" t="inlineStr"/>
@@ -22370,8 +22372,7 @@
       </c>
       <c r="C353" t="inlineStr">
         <is>
-          <t xml:space="preserve">UMC-1-Teste da orelhinha-U01-060
-</t>
+          <t>UMC-1-Teste da orelhinha-U01-060</t>
         </is>
       </c>
       <c r="D353" t="inlineStr">

</xml_diff>

<commit_message>
Foram simplificados alguns trechos para a documentação
</commit_message>
<xml_diff>
--- a/src/Ramais.xlsx
+++ b/src/Ramais.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O355"/>
+  <dimension ref="A1:O356"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22574,6 +22574,71 @@
         </is>
       </c>
     </row>
+    <row r="356">
+      <c r="A356" t="n">
+        <v>355</v>
+      </c>
+      <c r="B356" t="n">
+        <v>9999</v>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>example</t>
+        </is>
+      </c>
+      <c r="D356" t="inlineStr">
+        <is>
+          <t>example</t>
+        </is>
+      </c>
+      <c r="E356" t="inlineStr">
+        <is>
+          <t>GERÊNCIA</t>
+        </is>
+      </c>
+      <c r="F356" t="inlineStr">
+        <is>
+          <t>DIVISÃO</t>
+        </is>
+      </c>
+      <c r="G356" t="inlineStr">
+        <is>
+          <t>SETOR</t>
+        </is>
+      </c>
+      <c r="H356" t="inlineStr">
+        <is>
+          <t>UNIDADE</t>
+        </is>
+      </c>
+      <c r="I356" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="J356" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="K356" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="L356" t="inlineStr"/>
+      <c r="M356" t="inlineStr"/>
+      <c r="N356" t="inlineStr">
+        <is>
+          <t>19-05-25</t>
+        </is>
+      </c>
+      <c r="O356" t="inlineStr">
+        <is>
+          <t>Incluso na lista</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
[20/05/2025 - 09:37]Edições feitas para a documentação, foi feita simplificação de linhas e comentários para ficar mais entendível
</commit_message>
<xml_diff>
--- a/src/Ramais.xlsx
+++ b/src/Ramais.xlsx
@@ -1893,7 +1893,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Junio Eduvirgem</t>
+          <t>USID - Chefia</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -22450,11 +22450,7 @@
           <t>GERÊNCIA ADMINISTRATIVA</t>
         </is>
       </c>
-      <c r="F354" t="inlineStr">
-        <is>
-          <t>SEM DIVISÃO</t>
-        </is>
-      </c>
+      <c r="F354" t="inlineStr"/>
       <c r="G354" t="inlineStr">
         <is>
           <t xml:space="preserve">SUPORTE OPERACIONAL </t>
@@ -22523,11 +22519,7 @@
           <t>GERÊNCIA ADMINISTRATIVA</t>
         </is>
       </c>
-      <c r="F355" t="inlineStr">
-        <is>
-          <t>SEM DIVISÃO</t>
-        </is>
-      </c>
+      <c r="F355" t="inlineStr"/>
       <c r="G355" t="inlineStr">
         <is>
           <t xml:space="preserve">SUPORTE OPERACIONAL </t>

</xml_diff>